<commit_message>
update online training engine 23/12/15
</commit_message>
<xml_diff>
--- a/documents/tables.xlsx
+++ b/documents/tables.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kangpx/onlineTiny2023/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E269CACD-4CA7-9E46-BA13-3C804757BC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9807BCB9-2B03-CA41-9031-94EA69A1FD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{8810936B-8C3B-4749-9AC9-1596E102DCAF}"/>
+    <workbookView xWindow="2280" yWindow="2520" windowWidth="19200" windowHeight="18380" firstSheet="1" activeTab="3" xr2:uid="{8810936B-8C3B-4749-9AC9-1596E102DCAF}"/>
   </bookViews>
   <sheets>
     <sheet name="QVAR-c32-ADAM(0.002,0.9,0.999)" sheetId="3" r:id="rId1"/>
     <sheet name="QVAR-c32-ADAM(0.002,0.9,0.99)" sheetId="1" r:id="rId2"/>
     <sheet name="QVAR-c32-SGD(0.002,0.5)" sheetId="2" r:id="rId3"/>
+    <sheet name="Gym-b32-SGD(0.002,0.9)-norm" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="25">
   <si>
     <t>On GAP9 (GVSOC)</t>
   </si>
@@ -119,7 +120,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -284,6 +285,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -294,15 +304,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -621,25 +622,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC9FCB7-D2E0-7943-A41C-92F086194575}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" ht="46" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="A2" s="8"/>
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
@@ -657,16 +658,16 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="4">
         <v>0.7742</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="4">
         <v>0.99462399999999995</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="4">
         <v>0.76880000000000004</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="4">
         <v>0.97850000000000004</v>
       </c>
     </row>
@@ -674,16 +675,16 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="5">
         <v>0.80569999999999997</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="5">
         <v>0.91428600000000004</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="4">
         <v>0.80569999999999997</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="4">
         <v>0.94289999999999996</v>
       </c>
     </row>
@@ -691,16 +692,16 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="4">
         <v>0.58426999999999996</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="4">
         <v>0.79775300000000005</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="4">
         <v>0.58430000000000004</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="4">
         <v>0.89329999999999998</v>
       </c>
     </row>
@@ -708,16 +709,16 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="4">
         <v>0.39354800000000001</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="4">
         <v>0.72903200000000001</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="4">
         <v>0.4</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="4">
         <v>0.76770000000000005</v>
       </c>
     </row>
@@ -725,16 +726,16 @@
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="4">
         <v>0.53448300000000004</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="4">
         <v>0.89655200000000002</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>0.51719999999999999</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="4">
         <v>0.86209999999999998</v>
       </c>
     </row>
@@ -742,16 +743,16 @@
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="4">
         <v>0.48330000000000001</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="4">
         <v>0.9</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="4">
         <v>0.49440000000000001</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="4">
         <v>0.83330000000000004</v>
       </c>
     </row>
@@ -759,16 +760,16 @@
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="4">
         <v>0.64939999999999998</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="4">
         <v>0.83908000000000005</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="4">
         <v>0.64939999999999998</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="4">
         <v>0.82179999999999997</v>
       </c>
     </row>
@@ -776,16 +777,16 @@
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="4">
         <v>0.95</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="4">
         <v>0.98888900000000002</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="4">
         <v>0.95</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="4">
         <v>0.9778</v>
       </c>
     </row>
@@ -793,16 +794,16 @@
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="4">
         <v>0.89090000000000003</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="4">
         <v>0.95150000000000001</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="4">
         <v>0.88480000000000003</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="4">
         <v>0.94550000000000001</v>
       </c>
     </row>
@@ -810,16 +811,16 @@
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="4">
         <v>0.56799999999999995</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="4">
         <v>0.95266300000000004</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="4">
         <v>0.56799999999999995</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="4">
         <v>0.95860000000000001</v>
       </c>
     </row>
@@ -827,16 +828,16 @@
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="4">
         <v>0.88759999999999994</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="4">
         <v>0.94381999999999999</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="4">
         <v>0.88759999999999994</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="4">
         <v>0.92700000000000005</v>
       </c>
     </row>
@@ -844,16 +845,16 @@
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="4">
         <v>0.83330000000000004</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="4">
         <v>0.90555600000000003</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="4">
         <v>0.82779999999999998</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="4">
         <v>0.93889999999999996</v>
       </c>
     </row>
@@ -861,16 +862,16 @@
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="4">
         <v>0.85229999999999995</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="4">
         <v>0.90909099999999998</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="4">
         <v>0.84089999999999998</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="4">
         <v>0.88070000000000004</v>
       </c>
     </row>
@@ -878,16 +879,16 @@
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="4">
         <v>0.88</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="4">
         <v>0.89142900000000003</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="4">
         <v>0.87429999999999997</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="4">
         <v>0.94289999999999996</v>
       </c>
     </row>
@@ -895,16 +896,16 @@
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="4">
         <v>0.89329999999999998</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="4">
         <v>0.949438</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="4">
         <v>0.88759999999999994</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="4">
         <v>0.94379999999999997</v>
       </c>
     </row>
@@ -912,16 +913,16 @@
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="4">
         <v>0.53110000000000002</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="4">
         <v>0.83050800000000002</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="4">
         <v>0.52539999999999998</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="4">
         <v>0.83050000000000002</v>
       </c>
     </row>
@@ -929,16 +930,16 @@
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="4">
         <v>0.43180000000000002</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="4">
         <v>0.57575799999999999</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="4">
         <v>0.43940000000000001</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="4">
         <v>0.59089999999999998</v>
       </c>
     </row>
@@ -946,16 +947,16 @@
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="4">
         <v>0.50561800000000001</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="4">
         <v>0.81459999999999999</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="4">
         <v>0.5</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="4">
         <v>0.87639999999999996</v>
       </c>
     </row>
@@ -963,16 +964,16 @@
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="4">
         <v>0.64942500000000003</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="4">
         <v>0.72413799999999995</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="4">
         <v>0.64370000000000005</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="4">
         <v>0.77590000000000003</v>
       </c>
     </row>
@@ -980,16 +981,16 @@
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="6">
         <v>0.83522700000000005</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="6">
         <v>0.90909099999999998</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="6">
         <v>0.82389999999999997</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="6">
         <v>0.89200000000000002</v>
       </c>
     </row>
@@ -997,18 +998,18 @@
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="4">
         <f>AVERAGE(B3:B22)</f>
         <v>0.69667355000000009</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="4">
         <f>AVERAGE(C3:C22)</f>
         <v>0.87089040000000018</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="4">
         <v>0.69369999999999998</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="4">
         <v>0.879</v>
       </c>
     </row>
@@ -1039,18 +1040,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" ht="46" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="A2" s="8"/>
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1068,16 +1069,16 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="4">
         <v>0.7742</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="4">
         <v>0.96240000000000003</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="4">
         <v>0.76880000000000004</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="4">
         <v>0.97850000000000004</v>
       </c>
     </row>
@@ -1085,16 +1086,16 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="5">
         <v>0.80569999999999997</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="5">
         <v>0.92569999999999997</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="4">
         <v>0.80569999999999997</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="4">
         <v>0.94289999999999996</v>
       </c>
     </row>
@@ -1102,16 +1103,16 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="4">
         <v>0.58426999999999996</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="4">
         <v>0.85955099999999995</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="4">
         <v>0.58430000000000004</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="4">
         <v>0.91010000000000002</v>
       </c>
     </row>
@@ -1119,16 +1120,16 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="4">
         <v>0.39354800000000001</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="4">
         <v>0.69030000000000002</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="4">
         <v>0.4</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="4">
         <v>0.73550000000000004</v>
       </c>
     </row>
@@ -1136,16 +1137,16 @@
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="4">
         <v>0.53448300000000004</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="4">
         <v>0.89080000000000004</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>0.51719999999999999</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="4">
         <v>0.8851</v>
       </c>
     </row>
@@ -1153,16 +1154,16 @@
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="4">
         <v>0.48330000000000001</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="4">
         <v>0.91110000000000002</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="4">
         <v>0.49440000000000001</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="4">
         <v>0.85</v>
       </c>
     </row>
@@ -1170,16 +1171,16 @@
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="4">
         <v>0.64939999999999998</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="4">
         <v>0.82758600000000004</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="4">
         <v>0.64939999999999998</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="4">
         <v>0.81030000000000002</v>
       </c>
     </row>
@@ -1187,16 +1188,16 @@
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="4">
         <v>0.95</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="4">
         <v>0.98329999999999995</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="4">
         <v>0.95</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="4">
         <v>0.9778</v>
       </c>
     </row>
@@ -1204,16 +1205,16 @@
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="4">
         <v>0.89090000000000003</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="4">
         <v>0.96363600000000005</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="4">
         <v>0.88480000000000003</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="4">
         <v>0.95150000000000001</v>
       </c>
     </row>
@@ -1221,16 +1222,16 @@
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="4">
         <v>0.56799999999999995</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="4">
         <v>0.93491100000000005</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="4">
         <v>0.56799999999999995</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="4">
         <v>0.95269999999999999</v>
       </c>
     </row>
@@ -1238,16 +1239,16 @@
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="4">
         <v>0.88759999999999994</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="4">
         <v>0.87078599999999995</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="4">
         <v>0.88759999999999994</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="4">
         <v>0.92700000000000005</v>
       </c>
     </row>
@@ -1255,16 +1256,16 @@
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="4">
         <v>0.83330000000000004</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="4">
         <v>0.89439999999999997</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="4">
         <v>0.82779999999999998</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="4">
         <v>0.94440000000000002</v>
       </c>
     </row>
@@ -1272,16 +1273,16 @@
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="4">
         <v>0.85229999999999995</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="4">
         <v>0.89200000000000002</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="4">
         <v>0.84089999999999998</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="4">
         <v>0.88070000000000004</v>
       </c>
     </row>
@@ -1289,16 +1290,16 @@
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="4">
         <v>0.88</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="4">
         <v>0.88570000000000004</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="4">
         <v>0.87429999999999997</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="4">
         <v>0.94289999999999996</v>
       </c>
     </row>
@@ -1306,16 +1307,16 @@
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="4">
         <v>0.89329999999999998</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="4">
         <v>0.92700000000000005</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="4">
         <v>0.88759999999999994</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="4">
         <v>0.95509999999999995</v>
       </c>
     </row>
@@ -1323,16 +1324,16 @@
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="4">
         <v>0.53110000000000002</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="4">
         <v>0.83050000000000002</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="4">
         <v>0.52539999999999998</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="4">
         <v>0.84179999999999999</v>
       </c>
     </row>
@@ -1340,16 +1341,16 @@
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="4">
         <v>0.43180000000000002</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="4">
         <v>0.69699999999999995</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="4">
         <v>0.43940000000000001</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="4">
         <v>0.58330000000000004</v>
       </c>
     </row>
@@ -1357,16 +1358,16 @@
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="4">
         <v>0.50561800000000001</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="4">
         <v>0.93258399999999997</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="4">
         <v>0.5</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="4">
         <v>0.88200000000000001</v>
       </c>
     </row>
@@ -1374,16 +1375,16 @@
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="4">
         <v>0.64942500000000003</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="4">
         <v>0.76436800000000005</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="4">
         <v>0.64370000000000005</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="4">
         <v>0.79310000000000003</v>
       </c>
     </row>
@@ -1391,16 +1392,16 @@
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="6">
         <v>0.83522700000000005</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="6">
         <v>0.90340900000000002</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="6">
         <v>0.82389999999999997</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="6">
         <v>0.88639999999999997</v>
       </c>
     </row>
@@ -1408,18 +1409,18 @@
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="4">
         <f>AVERAGE(B3:B22)</f>
         <v>0.69667355000000009</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="4">
         <f>AVERAGE(C3:C22)</f>
         <v>0.87735154999999998</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="4">
         <v>0.69369999999999998</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="4">
         <v>0.88149999999999995</v>
       </c>
     </row>
@@ -1437,25 +1438,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25AFB81A-253C-784D-A2DE-906F12F7FD7F}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" ht="46" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="A2" s="8"/>
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1473,16 +1474,16 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="4">
         <v>0.7742</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="4">
         <v>0.98387100000000005</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="4">
         <v>0.76880000000000004</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="4">
         <v>0.97309999999999997</v>
       </c>
     </row>
@@ -1490,16 +1491,16 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="5">
         <v>0.80569999999999997</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="5">
         <v>0.90857100000000002</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="4">
         <v>0.80569999999999997</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="4">
         <v>0.93140000000000001</v>
       </c>
     </row>
@@ -1507,16 +1508,16 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="4">
         <v>0.58426999999999996</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="4">
         <v>0.85393300000000005</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="4">
         <v>0.58430000000000004</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="4">
         <v>0.84830000000000005</v>
       </c>
     </row>
@@ -1524,16 +1525,16 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="4">
         <v>0.39354800000000001</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="4">
         <v>0.73548400000000003</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="4">
         <v>0.4</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="4">
         <v>0.71609999999999996</v>
       </c>
     </row>
@@ -1541,16 +1542,16 @@
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="4">
         <v>0.53448300000000004</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="4">
         <v>0.88505699999999998</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>0.51719999999999999</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="4">
         <v>0.83909999999999996</v>
       </c>
     </row>
@@ -1558,16 +1559,16 @@
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="4">
         <v>0.48330000000000001</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="4">
         <v>0.88890000000000002</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="4">
         <v>0.49440000000000001</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="4">
         <v>0.8</v>
       </c>
     </row>
@@ -1575,16 +1576,16 @@
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="4">
         <v>0.64939999999999998</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="4">
         <v>0.81609200000000004</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="4">
         <v>0.64939999999999998</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="4">
         <v>0.78159999999999996</v>
       </c>
     </row>
@@ -1592,16 +1593,16 @@
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="4">
         <v>0.95</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="4">
         <v>0.97777000000000003</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="4">
         <v>0.95</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="4">
         <v>0.9667</v>
       </c>
     </row>
@@ -1609,16 +1610,16 @@
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="4">
         <v>0.89090000000000003</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="4">
         <v>0.95757599999999998</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="4">
         <v>0.88480000000000003</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="4">
         <v>0.93940000000000001</v>
       </c>
     </row>
@@ -1626,16 +1627,16 @@
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="4">
         <v>0.56799999999999995</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="4">
         <v>0.94674599999999998</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="4">
         <v>0.56799999999999995</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="4">
         <v>0.88759999999999994</v>
       </c>
     </row>
@@ -1643,16 +1644,16 @@
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="4">
         <v>0.88759999999999994</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="4">
         <v>0.92696599999999996</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="4">
         <v>0.88759999999999994</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="4">
         <v>0.91569999999999996</v>
       </c>
     </row>
@@ -1660,16 +1661,16 @@
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="4">
         <v>0.83330000000000004</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="4">
         <v>0.93330000000000002</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="4">
         <v>0.82779999999999998</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="4">
         <v>0.92220000000000002</v>
       </c>
     </row>
@@ -1677,16 +1678,16 @@
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="4">
         <v>0.85229999999999995</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="4">
         <v>0.89772700000000005</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="4">
         <v>0.84089999999999998</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="4">
         <v>0.89200000000000002</v>
       </c>
     </row>
@@ -1694,16 +1695,16 @@
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="4">
         <v>0.88</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="4">
         <v>0.88</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="4">
         <v>0.87429999999999997</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="4">
         <v>0.88570000000000004</v>
       </c>
     </row>
@@ -1711,16 +1712,16 @@
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="4">
         <v>0.89329999999999998</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="4">
         <v>0.96629200000000004</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="4">
         <v>0.88759999999999994</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="4">
         <v>0.94940000000000002</v>
       </c>
     </row>
@@ -1728,16 +1729,16 @@
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="4">
         <v>0.53110000000000002</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="4">
         <v>0.83615799999999996</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="4">
         <v>0.52539999999999998</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="4">
         <v>0.7853</v>
       </c>
     </row>
@@ -1745,16 +1746,16 @@
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="4">
         <v>0.43180000000000002</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="4">
         <v>0.62121199999999999</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="4">
         <v>0.43940000000000001</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="4">
         <v>0.54549999999999998</v>
       </c>
     </row>
@@ -1762,16 +1763,16 @@
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="4">
         <v>0.50561800000000001</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="4">
         <v>0.91011200000000003</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="4">
         <v>0.5</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="4">
         <v>0.82020000000000004</v>
       </c>
     </row>
@@ -1779,16 +1780,16 @@
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="4">
         <v>0.64942500000000003</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="4">
         <v>0.75862099999999999</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="4">
         <v>0.64370000000000005</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="4">
         <v>0.74139999999999995</v>
       </c>
     </row>
@@ -1796,16 +1797,16 @@
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="6">
         <v>0.83522700000000005</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="6">
         <v>0.91477299999999995</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="6">
         <v>0.82389999999999997</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="6">
         <v>0.89770000000000005</v>
       </c>
     </row>
@@ -1813,19 +1814,256 @@
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="4">
         <f>AVERAGE(B3:B22)</f>
         <v>0.69667355000000009</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="4">
         <f>AVERAGE(C3:C22)</f>
         <v>0.87995804999999994</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="4">
         <v>0.69369999999999998</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="4">
         <v>0.85189999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1060B3B9-9E53-734A-B1CE-BC197FFD7D29}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:5" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.94040000000000001</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.89670000000000005</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.94340000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.93730000000000002</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.93820000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.93389999999999995</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.95379999999999998</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.93159999999999998</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.95379999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.90410000000000001</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.86460000000000004</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.9073</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.91110000000000002</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.94679999999999997</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.91069999999999995</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.94969999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.90090000000000003</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.92630000000000001</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.90010000000000001</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.92949999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.88139999999999996</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.92889999999999995</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.88139999999999996</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.93530000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.91080000000000005</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.94810000000000005</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.90839999999999999</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.94920000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.90149999999999997</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.9335</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.90149999999999997</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.93889999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.92279999999999995</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.95620000000000005</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.92259999999999998</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.95940000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="4">
+        <f>AVERAGE(B3:B12)</f>
+        <v>0.90374000000000021</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" ref="C13:E13" si="0">AVERAGE(C3:C12)</f>
+        <v>0.93754000000000004</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="0"/>
+        <v>0.90305999999999997</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="0"/>
+        <v>0.94047000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>